<commit_message>
Update project files: analysis notebooks, data exports, and configurations
- Updated analysis notebooks (Hausman检验, Person, analyze, etc.)
- Added new export data files (量表数据, 多元线性回归数据)
- Updated data files and configurations
- Added project documentation (项目经历.md)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Administrator\Documents\大三下\标准化优秀毕业论文\期刊\数据\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837E8610-91F7-4185-A6CA-B86E7DE901D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3391771D-4295-4977-BB08-5DBF060CA31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>标准研制贡献指数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -151,11 +151,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -639,10 +642,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F222"/>
+  <dimension ref="A1:H222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -653,9 +656,10 @@
     <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="5" width="21.25" customWidth="1"/>
     <col min="6" max="6" width="29.75" customWidth="1"/>
+    <col min="7" max="7" width="19.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -674,13 +678,16 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>2006</v>
+      <c r="B2" s="2">
+        <v>39082</v>
       </c>
       <c r="C2">
         <v>65</v>
@@ -694,13 +701,16 @@
       <c r="F2">
         <v>151911</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G2" s="1">
+        <v>59.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>2007</v>
+      <c r="B3" s="2">
+        <v>39447</v>
       </c>
       <c r="C3">
         <v>51</v>
@@ -714,13 +724,16 @@
       <c r="F3">
         <v>196253</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G3" s="1">
+        <v>46.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>2008</v>
+      <c r="B4" s="2">
+        <v>39813</v>
       </c>
       <c r="C4">
         <v>188</v>
@@ -734,13 +747,16 @@
       <c r="F4">
         <v>237203</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G4" s="1">
+        <v>215.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>2009</v>
+      <c r="B5" s="2">
+        <v>40178</v>
       </c>
       <c r="C5">
         <v>89</v>
@@ -751,16 +767,19 @@
       <c r="E5">
         <v>56035</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F5" s="1">
+        <v>239199</v>
+      </c>
+      <c r="G5" s="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>2010</v>
+      <c r="B6" s="2">
+        <v>40543</v>
       </c>
       <c r="C6">
         <v>141</v>
@@ -774,13 +793,16 @@
       <c r="F6">
         <v>281601</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G6" s="1">
+        <v>101.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>2011</v>
+      <c r="B7" s="2">
+        <v>40908</v>
       </c>
       <c r="C7">
         <v>108</v>
@@ -794,13 +816,16 @@
       <c r="F7">
         <v>356588</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G7" s="1">
+        <v>122.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>2012</v>
+      <c r="B8" s="2">
+        <v>41274</v>
       </c>
       <c r="C8">
         <v>96</v>
@@ -814,13 +839,17 @@
       <c r="F8">
         <v>413031</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G8" s="1">
+        <v>94.3</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>2013</v>
+      <c r="B9" s="2">
+        <v>41639</v>
       </c>
       <c r="C9">
         <v>132</v>
@@ -834,13 +863,17 @@
       <c r="F9">
         <v>403262</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G9" s="1">
+        <v>115.8</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
-        <v>2014</v>
+      <c r="B10" s="2">
+        <v>42004</v>
       </c>
       <c r="C10">
         <v>132</v>
@@ -854,13 +887,17 @@
       <c r="F10">
         <v>329070</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G10" s="1">
+        <v>115.3</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B11">
-        <v>2015</v>
+      <c r="B11" s="2">
+        <v>42369</v>
       </c>
       <c r="C11">
         <v>127</v>
@@ -874,13 +911,17 @@
       <c r="F11">
         <v>333459</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G11" s="1">
+        <v>103.5</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B12">
-        <v>2016</v>
+      <c r="B12" s="2">
+        <v>42735</v>
       </c>
       <c r="C12">
         <v>97</v>
@@ -894,13 +935,16 @@
       <c r="F12">
         <v>347937</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G12" s="1">
+        <v>115.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="B13">
-        <v>2017</v>
+      <c r="B13" s="2">
+        <v>43100</v>
       </c>
       <c r="C13">
         <v>273</v>
@@ -914,13 +958,16 @@
       <c r="F13">
         <v>367273</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G13" s="1">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B14">
-        <v>2018</v>
+      <c r="B14" s="2">
+        <v>43465</v>
       </c>
       <c r="C14">
         <v>196</v>
@@ -934,13 +981,16 @@
       <c r="F14">
         <v>385339</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G14" s="1">
+        <v>143.80000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>7</v>
       </c>
-      <c r="B15">
-        <v>2019</v>
+      <c r="B15" s="2">
+        <v>43830</v>
       </c>
       <c r="C15">
         <v>172</v>
@@ -954,13 +1004,16 @@
       <c r="F15">
         <v>410058</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G15" s="1">
+        <v>135.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B16">
-        <v>2020</v>
+      <c r="B16" s="2">
+        <v>44196</v>
       </c>
       <c r="C16">
         <v>241</v>
@@ -974,13 +1027,16 @@
       <c r="F16">
         <v>451504</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G16" s="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>7</v>
       </c>
-      <c r="B17">
-        <v>2021</v>
+      <c r="B17" s="2">
+        <v>44561</v>
       </c>
       <c r="C17">
         <v>274</v>
@@ -994,13 +1050,16 @@
       <c r="F17">
         <v>501445</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G17" s="1">
+        <v>167.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>7</v>
       </c>
-      <c r="B18">
-        <v>2022</v>
+      <c r="B18" s="2">
+        <v>44926</v>
       </c>
       <c r="C18">
         <v>302</v>
@@ -1014,13 +1073,16 @@
       <c r="F18">
         <v>484950</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G18" s="1">
+        <v>159.69999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19">
-        <v>2006</v>
+      <c r="B19" s="2">
+        <v>39082</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -1034,13 +1096,16 @@
       <c r="F19">
         <v>275228</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G19" s="1">
+        <v>26.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>12</v>
       </c>
-      <c r="B20">
-        <v>2007</v>
+      <c r="B20" s="2">
+        <v>39447</v>
       </c>
       <c r="C20">
         <v>20</v>
@@ -1054,13 +1119,16 @@
       <c r="F20">
         <v>277177</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G20" s="1">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>12</v>
       </c>
-      <c r="B21">
-        <v>2008</v>
+      <c r="B21" s="2">
+        <v>39813</v>
       </c>
       <c r="C21">
         <v>103</v>
@@ -1074,13 +1142,16 @@
       <c r="F21">
         <v>316651</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G21">
+        <v>141.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>12</v>
       </c>
-      <c r="B22">
-        <v>2009</v>
+      <c r="B22" s="2">
+        <v>40178</v>
       </c>
       <c r="C22">
         <v>56</v>
@@ -1094,13 +1165,16 @@
       <c r="F22">
         <v>320308</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G22">
+        <v>97.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>12</v>
       </c>
-      <c r="B23">
-        <v>2010</v>
+      <c r="B23" s="2">
+        <v>40543</v>
       </c>
       <c r="C23">
         <v>49</v>
@@ -1114,13 +1188,16 @@
       <c r="F23">
         <v>330007</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G23">
+        <v>58.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>12</v>
       </c>
-      <c r="B24">
-        <v>2011</v>
+      <c r="B24" s="2">
+        <v>40908</v>
       </c>
       <c r="C24">
         <v>43</v>
@@ -1134,13 +1211,16 @@
       <c r="F24">
         <v>350480</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G24">
+        <v>48.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>12</v>
       </c>
-      <c r="B25">
-        <v>2012</v>
+      <c r="B25" s="2">
+        <v>41274</v>
       </c>
       <c r="C25">
         <v>50</v>
@@ -1154,13 +1234,16 @@
       <c r="F25">
         <v>400953</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G25">
+        <v>57.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>12</v>
       </c>
-      <c r="B26">
-        <v>2013</v>
+      <c r="B26" s="2">
+        <v>41639</v>
       </c>
       <c r="C26">
         <v>53</v>
@@ -1174,13 +1257,16 @@
       <c r="F26">
         <v>333886</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G26">
+        <v>61.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>12</v>
       </c>
-      <c r="B27">
-        <v>2014</v>
+      <c r="B27" s="2">
+        <v>42004</v>
       </c>
       <c r="C27">
         <v>41</v>
@@ -1194,13 +1280,16 @@
       <c r="F27">
         <v>290438</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G27">
+        <v>44.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>12</v>
       </c>
-      <c r="B28">
-        <v>2015</v>
+      <c r="B28" s="2">
+        <v>42369</v>
       </c>
       <c r="C28">
         <v>44</v>
@@ -1214,13 +1303,16 @@
       <c r="F28">
         <v>320219</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G28">
+        <v>71.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>12</v>
       </c>
-      <c r="B29">
-        <v>2016</v>
+      <c r="B29" s="2">
+        <v>42735</v>
       </c>
       <c r="C29">
         <v>41</v>
@@ -1234,13 +1326,16 @@
       <c r="F29">
         <v>341273</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G29">
+        <v>58.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>12</v>
       </c>
-      <c r="B30">
-        <v>2017</v>
+      <c r="B30" s="2">
+        <v>43100</v>
       </c>
       <c r="C30">
         <v>109</v>
@@ -1254,13 +1349,16 @@
       <c r="F30">
         <v>367545</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G30">
+        <v>111.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>12</v>
       </c>
-      <c r="B31">
-        <v>2018</v>
+      <c r="B31" s="2">
+        <v>43465</v>
       </c>
       <c r="C31">
         <v>84</v>
@@ -1274,13 +1372,16 @@
       <c r="F31">
         <v>369133</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G31">
+        <v>81.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>12</v>
       </c>
-      <c r="B32">
-        <v>2019</v>
+      <c r="B32" s="2">
+        <v>43830</v>
       </c>
       <c r="C32">
         <v>72</v>
@@ -1294,13 +1395,16 @@
       <c r="F32">
         <v>361977</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G32">
+        <v>81.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>12</v>
       </c>
-      <c r="B33">
-        <v>2020</v>
+      <c r="B33" s="2">
+        <v>44196</v>
       </c>
       <c r="C33">
         <v>98</v>
@@ -1314,13 +1418,16 @@
       <c r="F33">
         <v>362107</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G33">
+        <v>90.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>12</v>
       </c>
-      <c r="B34">
-        <v>2021</v>
+      <c r="B34" s="2">
+        <v>44561</v>
       </c>
       <c r="C34">
         <v>101</v>
@@ -1334,13 +1441,16 @@
       <c r="F34">
         <v>380714</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G34">
+        <v>91.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>12</v>
       </c>
-      <c r="B35">
-        <v>2022</v>
+      <c r="B35" s="2">
+        <v>44926</v>
       </c>
       <c r="C35">
         <v>144</v>
@@ -1354,13 +1464,16 @@
       <c r="F35">
         <v>382613</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G35">
+        <v>102.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>13</v>
       </c>
-      <c r="B36">
-        <v>2006</v>
+      <c r="B36" s="2">
+        <v>39082</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1374,13 +1487,16 @@
       <c r="F36">
         <v>24433</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G36">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>13</v>
       </c>
-      <c r="B37">
-        <v>2007</v>
+      <c r="B37" s="2">
+        <v>39447</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1394,13 +1510,16 @@
       <c r="F37">
         <v>44290</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G37">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>13</v>
       </c>
-      <c r="B38">
-        <v>2008</v>
+      <c r="B38" s="2">
+        <v>39813</v>
       </c>
       <c r="C38">
         <v>11</v>
@@ -1414,13 +1533,16 @@
       <c r="F38">
         <v>58251</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G38">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>13</v>
       </c>
-      <c r="B39">
-        <v>2009</v>
+      <c r="B39" s="2">
+        <v>40178</v>
       </c>
       <c r="C39">
         <v>15</v>
@@ -1434,13 +1556,16 @@
       <c r="F39">
         <v>69781</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G39">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>13</v>
       </c>
-      <c r="B40">
-        <v>2010</v>
+      <c r="B40" s="2">
+        <v>40543</v>
       </c>
       <c r="C40">
         <v>18</v>
@@ -1454,13 +1579,16 @@
       <c r="F40">
         <v>101330</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G40">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>13</v>
       </c>
-      <c r="B41">
-        <v>2011</v>
+      <c r="B41" s="2">
+        <v>40908</v>
       </c>
       <c r="C41">
         <v>5</v>
@@ -1474,13 +1602,16 @@
       <c r="F41">
         <v>146569</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>13</v>
       </c>
-      <c r="B42">
-        <v>2012</v>
+      <c r="B42" s="2">
+        <v>41274</v>
       </c>
       <c r="C42">
         <v>8</v>
@@ -1494,13 +1625,16 @@
       <c r="F42">
         <v>170021</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>13</v>
       </c>
-      <c r="B43">
-        <v>2013</v>
+      <c r="B43" s="2">
+        <v>41639</v>
       </c>
       <c r="C43">
         <v>9</v>
@@ -1514,13 +1648,16 @@
       <c r="F43">
         <v>150047</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G43">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>13</v>
       </c>
-      <c r="B44">
-        <v>2014</v>
+      <c r="B44" s="2">
+        <v>42004</v>
       </c>
       <c r="C44">
         <v>14</v>
@@ -1534,13 +1671,16 @@
       <c r="F44">
         <v>165786</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G44">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>13</v>
       </c>
-      <c r="B45">
-        <v>2015</v>
+      <c r="B45" s="2">
+        <v>42369</v>
       </c>
       <c r="C45">
         <v>14</v>
@@ -1554,13 +1694,16 @@
       <c r="F45">
         <v>142788</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G45">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>13</v>
       </c>
-      <c r="B46">
-        <v>2016</v>
+      <c r="B46" s="2">
+        <v>42735</v>
       </c>
       <c r="C46">
         <v>17</v>
@@ -1574,13 +1717,16 @@
       <c r="F46">
         <v>150574</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G46">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>13</v>
       </c>
-      <c r="B47">
-        <v>2017</v>
+      <c r="B47" s="2">
+        <v>43100</v>
       </c>
       <c r="C47">
         <v>28</v>
@@ -1594,13 +1740,16 @@
       <c r="F47">
         <v>165991</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G47">
+        <v>34.700000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>13</v>
       </c>
-      <c r="B48">
-        <v>2018</v>
+      <c r="B48" s="2">
+        <v>43465</v>
       </c>
       <c r="C48">
         <v>21</v>
@@ -1614,13 +1763,16 @@
       <c r="F48">
         <v>189848</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G48">
+        <v>22.3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>13</v>
       </c>
-      <c r="B49">
-        <v>2019</v>
+      <c r="B49" s="2">
+        <v>43830</v>
       </c>
       <c r="C49">
         <v>14</v>
@@ -1634,13 +1786,16 @@
       <c r="F49">
         <v>208997</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G49">
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>13</v>
       </c>
-      <c r="B50">
-        <v>2020</v>
+      <c r="B50" s="2">
+        <v>44196</v>
       </c>
       <c r="C50">
         <v>27</v>
@@ -1654,13 +1809,16 @@
       <c r="F50">
         <v>220059</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G50">
+        <v>19.600000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>13</v>
       </c>
-      <c r="B51">
-        <v>2021</v>
+      <c r="B51" s="2">
+        <v>44561</v>
       </c>
       <c r="C51">
         <v>49</v>
@@ -1674,13 +1832,16 @@
       <c r="F51">
         <v>242250</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G51">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>13</v>
       </c>
-      <c r="B52">
-        <v>2022</v>
+      <c r="B52" s="2">
+        <v>44926</v>
       </c>
       <c r="C52">
         <v>42</v>
@@ -1694,13 +1855,16 @@
       <c r="F52">
         <v>122439</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G52">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>4</v>
       </c>
-      <c r="B53">
-        <v>2006</v>
+      <c r="B53" s="2">
+        <v>39082</v>
       </c>
       <c r="C53">
         <v>19</v>
@@ -1714,13 +1878,16 @@
       <c r="F53">
         <v>125145</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G53">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>4</v>
       </c>
-      <c r="B54">
-        <v>2007</v>
+      <c r="B54" s="2">
+        <v>39447</v>
       </c>
       <c r="C54">
         <v>29</v>
@@ -1734,13 +1901,16 @@
       <c r="F54">
         <v>183481</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G54">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>4</v>
       </c>
-      <c r="B55">
-        <v>2008</v>
+      <c r="B55" s="2">
+        <v>39813</v>
       </c>
       <c r="C55">
         <v>109</v>
@@ -1754,13 +1924,16 @@
       <c r="F55">
         <v>204002</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G55">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>4</v>
       </c>
-      <c r="B56">
-        <v>2009</v>
+      <c r="B56" s="2">
+        <v>40178</v>
       </c>
       <c r="C56">
         <v>79</v>
@@ -1774,13 +1947,16 @@
       <c r="F56">
         <v>258199</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G56">
+        <v>89.3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>4</v>
       </c>
-      <c r="B57">
-        <v>2010</v>
+      <c r="B57" s="2">
+        <v>40543</v>
       </c>
       <c r="C57">
         <v>60</v>
@@ -1794,13 +1970,16 @@
       <c r="F57">
         <v>267000</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G57">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>4</v>
       </c>
-      <c r="B58">
-        <v>2011</v>
+      <c r="B58" s="2">
+        <v>40908</v>
       </c>
       <c r="C58">
         <v>39</v>
@@ -1814,13 +1993,16 @@
       <c r="F58">
         <v>305238</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G58">
+        <v>39.1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>4</v>
       </c>
-      <c r="B59">
-        <v>2012</v>
+      <c r="B59" s="2">
+        <v>41274</v>
       </c>
       <c r="C59">
         <v>25</v>
@@ -1834,13 +2016,16 @@
       <c r="F59">
         <v>336073</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G59">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>4</v>
       </c>
-      <c r="B60">
-        <v>2013</v>
+      <c r="B60" s="2">
+        <v>41639</v>
       </c>
       <c r="C60">
         <v>36</v>
@@ -1854,13 +2039,16 @@
       <c r="F60">
         <v>353000</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G60">
+        <v>28.3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>4</v>
       </c>
-      <c r="B61">
-        <v>2014</v>
+      <c r="B61" s="2">
+        <v>42004</v>
       </c>
       <c r="C61">
         <v>41</v>
@@ -1874,13 +2062,16 @@
       <c r="F61">
         <v>240919</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G61">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>4</v>
       </c>
-      <c r="B62">
-        <v>2015</v>
+      <c r="B62" s="2">
+        <v>42369</v>
       </c>
       <c r="C62">
         <v>66</v>
@@ -1894,13 +2085,16 @@
       <c r="F62">
         <v>172065</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G62">
+        <v>66.099999999999994</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>4</v>
       </c>
-      <c r="B63">
-        <v>2016</v>
+      <c r="B63" s="2">
+        <v>42735</v>
       </c>
       <c r="C63">
         <v>23</v>
@@ -1914,13 +2108,16 @@
       <c r="F63">
         <v>250020</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G63">
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>4</v>
       </c>
-      <c r="B64">
-        <v>2017</v>
+      <c r="B64" s="2">
+        <v>43100</v>
       </c>
       <c r="C64">
         <v>95</v>
@@ -1934,13 +2131,16 @@
       <c r="F64">
         <v>221608</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G64">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>4</v>
       </c>
-      <c r="B65">
-        <v>2018</v>
+      <c r="B65" s="2">
+        <v>43465</v>
       </c>
       <c r="C65">
         <v>52</v>
@@ -1954,13 +2154,16 @@
       <c r="F65">
         <v>242189</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G65">
+        <v>49.2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
         <v>4</v>
       </c>
-      <c r="B66">
-        <v>2019</v>
+      <c r="B66" s="2">
+        <v>43830</v>
       </c>
       <c r="C66">
         <v>74</v>
@@ -1974,13 +2177,16 @@
       <c r="F66">
         <v>262812</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G66">
+        <v>57.7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
         <v>4</v>
       </c>
-      <c r="B67">
-        <v>2020</v>
+      <c r="B67" s="2">
+        <v>44196</v>
       </c>
       <c r="C67">
         <v>81</v>
@@ -1994,13 +2200,16 @@
       <c r="F67">
         <v>287838</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G67">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>4</v>
       </c>
-      <c r="B68">
-        <v>2021</v>
+      <c r="B68" s="2">
+        <v>44561</v>
       </c>
       <c r="C68">
         <v>103</v>
@@ -2014,13 +2223,16 @@
       <c r="F68">
         <v>307147</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G68">
+        <v>59.9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
         <v>4</v>
       </c>
-      <c r="B69">
-        <v>2022</v>
+      <c r="B69" s="2">
+        <v>44926</v>
       </c>
       <c r="C69">
         <v>104</v>
@@ -2034,13 +2246,16 @@
       <c r="F69">
         <v>283099</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G69">
+        <v>47.3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
         <v>9</v>
       </c>
-      <c r="B70">
-        <v>2006</v>
+      <c r="B70" s="2">
+        <v>39082</v>
       </c>
       <c r="C70">
         <v>16</v>
@@ -2054,13 +2269,16 @@
       <c r="F70">
         <v>610461</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G70">
+        <v>31.1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>9</v>
       </c>
-      <c r="B71">
-        <v>2007</v>
+      <c r="B71" s="2">
+        <v>39447</v>
       </c>
       <c r="C71">
         <v>41</v>
@@ -2074,13 +2292,16 @@
       <c r="F71">
         <v>716471</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G71">
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
         <v>9</v>
       </c>
-      <c r="B72">
-        <v>2008</v>
+      <c r="B72" s="2">
+        <v>39813</v>
       </c>
       <c r="C72">
         <v>73</v>
@@ -2094,13 +2315,16 @@
       <c r="F72">
         <v>813262</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G72">
+        <v>134.80000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
         <v>9</v>
       </c>
-      <c r="B73">
-        <v>2009</v>
+      <c r="B73" s="2">
+        <v>40178</v>
       </c>
       <c r="C73">
         <v>85</v>
@@ -2114,13 +2338,16 @@
       <c r="F73">
         <v>822653</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G73">
+        <v>132.4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
         <v>9</v>
       </c>
-      <c r="B74">
-        <v>2010</v>
+      <c r="B74" s="2">
+        <v>40543</v>
       </c>
       <c r="C74">
         <v>48</v>
@@ -2134,13 +2361,16 @@
       <c r="F74">
         <v>853511</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G74">
+        <v>96.3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>9</v>
       </c>
-      <c r="B75">
-        <v>2011</v>
+      <c r="B75" s="2">
+        <v>40908</v>
       </c>
       <c r="C75">
         <v>36</v>
@@ -2154,13 +2384,16 @@
       <c r="F75">
         <v>901623</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G75">
+        <v>97.3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
         <v>9</v>
       </c>
-      <c r="B76">
-        <v>2012</v>
+      <c r="B76" s="2">
+        <v>41274</v>
       </c>
       <c r="C76">
         <v>57</v>
@@ -2174,13 +2407,16 @@
       <c r="F76">
         <v>916490</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G76">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>9</v>
       </c>
-      <c r="B77">
-        <v>2013</v>
+      <c r="B77" s="2">
+        <v>41639</v>
       </c>
       <c r="C77">
         <v>62</v>
@@ -2194,13 +2430,16 @@
       <c r="F77">
         <v>869805</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G77">
+        <v>103.9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
         <v>9</v>
       </c>
-      <c r="B78">
-        <v>2014</v>
+      <c r="B78" s="2">
+        <v>42004</v>
       </c>
       <c r="C78">
         <v>55</v>
@@ -2214,13 +2453,16 @@
       <c r="F78">
         <v>811978</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G78">
+        <v>81.7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
         <v>9</v>
       </c>
-      <c r="B79">
-        <v>2015</v>
+      <c r="B79" s="2">
+        <v>42369</v>
       </c>
       <c r="C79">
         <v>83</v>
@@ -2234,13 +2476,16 @@
       <c r="F79">
         <v>600023</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G79">
+        <v>101.3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
         <v>9</v>
       </c>
-      <c r="B80">
-        <v>2016</v>
+      <c r="B80" s="2">
+        <v>42735</v>
       </c>
       <c r="C80">
         <v>71</v>
@@ -2254,13 +2499,16 @@
       <c r="F80">
         <v>600300</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G80">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
         <v>9</v>
       </c>
-      <c r="B81">
-        <v>2017</v>
+      <c r="B81" s="2">
+        <v>43100</v>
       </c>
       <c r="C81">
         <v>226</v>
@@ -2274,13 +2522,16 @@
       <c r="F81">
         <v>450392</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G81">
+        <v>243.3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
         <v>9</v>
       </c>
-      <c r="B82">
-        <v>2018</v>
+      <c r="B82" s="2">
+        <v>43465</v>
       </c>
       <c r="C82">
         <v>150</v>
@@ -2294,13 +2545,16 @@
       <c r="F82">
         <v>452498</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G82">
+        <v>180.6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>9</v>
       </c>
-      <c r="B83">
-        <v>2019</v>
+      <c r="B83" s="2">
+        <v>43830</v>
       </c>
       <c r="C83">
         <v>169</v>
@@ -2314,13 +2568,16 @@
       <c r="F83">
         <v>461545</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G83">
+        <v>174.4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
         <v>9</v>
       </c>
-      <c r="B84">
-        <v>2020</v>
+      <c r="B84" s="2">
+        <v>44196</v>
       </c>
       <c r="C84">
         <v>153</v>
@@ -2334,13 +2591,16 @@
       <c r="F84">
         <v>554030</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G84">
+        <v>184.6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>9</v>
       </c>
-      <c r="B85">
-        <v>2021</v>
+      <c r="B85" s="2">
+        <v>44561</v>
       </c>
       <c r="C85">
         <v>235</v>
@@ -2354,13 +2614,16 @@
       <c r="F85">
         <v>699218</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G85">
+        <v>275.60000000000002</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
         <v>9</v>
       </c>
-      <c r="B86">
-        <v>2022</v>
+      <c r="B86" s="2">
+        <v>44926</v>
       </c>
       <c r="C86">
         <v>283</v>
@@ -2374,13 +2637,16 @@
       <c r="F86">
         <v>741798</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G86">
+        <v>246.2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
         <v>8</v>
       </c>
-      <c r="B87">
-        <v>2006</v>
+      <c r="B87" s="2">
+        <v>39082</v>
       </c>
       <c r="C87">
         <v>4</v>
@@ -2394,13 +2660,16 @@
       <c r="F87">
         <v>257497</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G87">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
         <v>8</v>
       </c>
-      <c r="B88">
-        <v>2007</v>
+      <c r="B88" s="2">
+        <v>39447</v>
       </c>
       <c r="C88">
         <v>2</v>
@@ -2414,13 +2683,16 @@
       <c r="F88">
         <v>311745</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G88">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
         <v>8</v>
       </c>
-      <c r="B89">
-        <v>2008</v>
+      <c r="B89" s="2">
+        <v>39813</v>
       </c>
       <c r="C89">
         <v>16</v>
@@ -2434,13 +2706,16 @@
       <c r="F89">
         <v>293710</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G89">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
         <v>8</v>
       </c>
-      <c r="B90">
-        <v>2009</v>
+      <c r="B90" s="2">
+        <v>40178</v>
       </c>
       <c r="C90">
         <v>23</v>
@@ -2454,13 +2729,16 @@
       <c r="F90">
         <v>200481</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G90">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
         <v>8</v>
       </c>
-      <c r="B91">
-        <v>2010</v>
+      <c r="B91" s="2">
+        <v>40543</v>
       </c>
       <c r="C91">
         <v>8</v>
@@ -2474,13 +2752,16 @@
       <c r="F91">
         <v>206056</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G91">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
         <v>8</v>
       </c>
-      <c r="B92">
-        <v>2011</v>
+      <c r="B92" s="2">
+        <v>40908</v>
       </c>
       <c r="C92">
         <v>8</v>
@@ -2494,13 +2775,16 @@
       <c r="F92">
         <v>216644</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G92">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
         <v>8</v>
       </c>
-      <c r="B93">
-        <v>2012</v>
+      <c r="B93" s="2">
+        <v>41274</v>
       </c>
       <c r="C93">
         <v>12</v>
@@ -2514,13 +2798,16 @@
       <c r="F93">
         <v>220542</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G93">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
         <v>8</v>
       </c>
-      <c r="B94">
-        <v>2013</v>
+      <c r="B94" s="2">
+        <v>41639</v>
       </c>
       <c r="C94">
         <v>21</v>
@@ -2534,13 +2821,16 @@
       <c r="F94">
         <v>228743</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G94">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
         <v>8</v>
       </c>
-      <c r="B95">
-        <v>2014</v>
+      <c r="B95" s="2">
+        <v>42004</v>
       </c>
       <c r="C95">
         <v>16</v>
@@ -2554,13 +2844,16 @@
       <c r="F95">
         <v>230479</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G95">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
         <v>8</v>
       </c>
-      <c r="B96">
-        <v>2015</v>
+      <c r="B96" s="2">
+        <v>42369</v>
       </c>
       <c r="C96">
         <v>16</v>
@@ -2574,13 +2867,16 @@
       <c r="F96">
         <v>231559</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G96">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
         <v>8</v>
       </c>
-      <c r="B97">
-        <v>2016</v>
+      <c r="B97" s="2">
+        <v>42735</v>
       </c>
       <c r="C97">
         <v>11</v>
@@ -2594,13 +2890,16 @@
       <c r="F97">
         <v>238724</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G97">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
         <v>8</v>
       </c>
-      <c r="B98">
-        <v>2017</v>
+      <c r="B98" s="2">
+        <v>43100</v>
       </c>
       <c r="C98">
         <v>33</v>
@@ -2614,13 +2913,16 @@
       <c r="F98">
         <v>242266</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G98">
+        <v>37.9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
         <v>8</v>
       </c>
-      <c r="B99">
-        <v>2018</v>
+      <c r="B99" s="2">
+        <v>43465</v>
       </c>
       <c r="C99">
         <v>36</v>
@@ -2634,13 +2936,16 @@
       <c r="F99">
         <v>258140</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G99">
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
         <v>8</v>
       </c>
-      <c r="B100">
-        <v>2019</v>
+      <c r="B100" s="2">
+        <v>43830</v>
       </c>
       <c r="C100">
         <v>31</v>
@@ -2654,13 +2959,16 @@
       <c r="F100">
         <v>266528</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G100">
+        <v>24.9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
         <v>8</v>
       </c>
-      <c r="B101">
-        <v>2020</v>
+      <c r="B101" s="2">
+        <v>44196</v>
       </c>
       <c r="C101">
         <v>24</v>
@@ -2674,13 +2982,16 @@
       <c r="F101">
         <v>271248</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G101">
+        <v>30.8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
         <v>8</v>
       </c>
-      <c r="B102">
-        <v>2021</v>
+      <c r="B102" s="2">
+        <v>44561</v>
       </c>
       <c r="C102">
         <v>30</v>
@@ -2694,13 +3005,16 @@
       <c r="F102">
         <v>312093</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G102">
+        <v>39.1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
         <v>8</v>
       </c>
-      <c r="B103">
-        <v>2022</v>
+      <c r="B103" s="2">
+        <v>44926</v>
       </c>
       <c r="C103">
         <v>40</v>
@@ -2714,13 +3028,16 @@
       <c r="F103">
         <v>295178</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G103">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
         <v>6</v>
       </c>
-      <c r="B104">
-        <v>2006</v>
+      <c r="B104" s="2">
+        <v>39082</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -2734,13 +3051,16 @@
       <c r="F104">
         <v>34558</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
         <v>6</v>
       </c>
-      <c r="B105">
-        <v>2007</v>
+      <c r="B105" s="2">
+        <v>39447</v>
       </c>
       <c r="C105">
         <v>3</v>
@@ -2754,13 +3074,16 @@
       <c r="F105">
         <v>73787</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G105">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
         <v>6</v>
       </c>
-      <c r="B106">
-        <v>2008</v>
+      <c r="B106" s="2">
+        <v>39813</v>
       </c>
       <c r="C106">
         <v>5</v>
@@ -2774,13 +3097,16 @@
       <c r="F106">
         <v>93528</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G106">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
         <v>6</v>
       </c>
-      <c r="B107">
-        <v>2009</v>
+      <c r="B107" s="2">
+        <v>40178</v>
       </c>
       <c r="C107">
         <v>5</v>
@@ -2794,13 +3120,16 @@
       <c r="F107">
         <v>103992</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G107">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
         <v>6</v>
       </c>
-      <c r="B108">
-        <v>2010</v>
+      <c r="B108" s="2">
+        <v>40543</v>
       </c>
       <c r="C108">
         <v>2</v>
@@ -2814,13 +3143,16 @@
       <c r="F108">
         <v>110116</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G108">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
         <v>6</v>
       </c>
-      <c r="B109">
-        <v>2011</v>
+      <c r="B109" s="2">
+        <v>40908</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -2834,13 +3166,16 @@
       <c r="F109">
         <v>60986</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G109">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
         <v>6</v>
       </c>
-      <c r="B110">
-        <v>2012</v>
+      <c r="B110" s="2">
+        <v>41274</v>
       </c>
       <c r="C110">
         <v>1</v>
@@ -2854,13 +3189,16 @@
       <c r="F110">
         <v>73354</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
         <v>6</v>
       </c>
-      <c r="B111">
-        <v>2013</v>
+      <c r="B111" s="2">
+        <v>41639</v>
       </c>
       <c r="C111">
         <v>3</v>
@@ -2874,13 +3212,16 @@
       <c r="F111">
         <v>86990</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
         <v>6</v>
       </c>
-      <c r="B112">
-        <v>2014</v>
+      <c r="B112" s="2">
+        <v>42004</v>
       </c>
       <c r="C112">
         <v>2</v>
@@ -2894,13 +3235,16 @@
       <c r="F112">
         <v>95438</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G112">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
         <v>6</v>
       </c>
-      <c r="B113">
-        <v>2015</v>
+      <c r="B113" s="2">
+        <v>42369</v>
       </c>
       <c r="C113">
         <v>1</v>
@@ -2914,13 +3258,16 @@
       <c r="F113">
         <v>80108</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G113">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
         <v>6</v>
       </c>
-      <c r="B114">
-        <v>2016</v>
+      <c r="B114" s="2">
+        <v>42735</v>
       </c>
       <c r="C114">
         <v>1</v>
@@ -2934,13 +3281,16 @@
       <c r="F114">
         <v>55044</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G114">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
         <v>6</v>
       </c>
-      <c r="B115">
-        <v>2017</v>
+      <c r="B115" s="2">
+        <v>43100</v>
       </c>
       <c r="C115">
         <v>4</v>
@@ -2954,13 +3304,16 @@
       <c r="F115">
         <v>70902</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G115">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
         <v>6</v>
       </c>
-      <c r="B116">
-        <v>2018</v>
+      <c r="B116" s="2">
+        <v>43465</v>
       </c>
       <c r="C116">
         <v>16</v>
@@ -2974,13 +3327,16 @@
       <c r="F116">
         <v>60345</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G116">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
         <v>6</v>
       </c>
-      <c r="B117">
-        <v>2019</v>
+      <c r="B117" s="2">
+        <v>43830</v>
       </c>
       <c r="C117">
         <v>7</v>
@@ -2994,13 +3350,16 @@
       <c r="F117">
         <v>61402</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G117">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
         <v>6</v>
       </c>
-      <c r="B118">
-        <v>2020</v>
+      <c r="B118" s="2">
+        <v>44196</v>
       </c>
       <c r="C118">
         <v>7</v>
@@ -3014,13 +3373,16 @@
       <c r="F118">
         <v>67645</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G118">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
         <v>6</v>
       </c>
-      <c r="B119">
-        <v>2021</v>
+      <c r="B119" s="2">
+        <v>44561</v>
       </c>
       <c r="C119">
         <v>15</v>
@@ -3034,13 +3396,16 @@
       <c r="F119">
         <v>82430</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G119">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
         <v>6</v>
       </c>
-      <c r="B120">
-        <v>2022</v>
+      <c r="B120" s="2">
+        <v>44926</v>
       </c>
       <c r="C120">
         <v>10</v>
@@ -3054,13 +3419,16 @@
       <c r="F120">
         <v>78037</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G120">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
         <v>5</v>
       </c>
-      <c r="B121">
-        <v>2006</v>
+      <c r="B121" s="2">
+        <v>39082</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -3074,13 +3442,16 @@
       <c r="F121">
         <v>11569</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
         <v>5</v>
       </c>
-      <c r="B122">
-        <v>2007</v>
+      <c r="B122" s="2">
+        <v>39447</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -3094,13 +3465,16 @@
       <c r="F122">
         <v>28637</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G122">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
         <v>5</v>
       </c>
-      <c r="B123">
-        <v>2008</v>
+      <c r="B123" s="2">
+        <v>39813</v>
       </c>
       <c r="C123">
         <v>1</v>
@@ -3114,13 +3488,16 @@
       <c r="F123">
         <v>45465</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G123">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
         <v>5</v>
       </c>
-      <c r="B124">
-        <v>2009</v>
+      <c r="B124" s="2">
+        <v>40178</v>
       </c>
       <c r="C124">
         <v>1</v>
@@ -3134,13 +3511,16 @@
       <c r="F124">
         <v>61418</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G124">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
         <v>5</v>
       </c>
-      <c r="B125">
-        <v>2010</v>
+      <c r="B125" s="2">
+        <v>40543</v>
       </c>
       <c r="C125">
         <v>1</v>
@@ -3154,13 +3534,16 @@
       <c r="F125">
         <v>105153</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G125">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
         <v>5</v>
       </c>
-      <c r="B126">
-        <v>2011</v>
+      <c r="B126" s="2">
+        <v>40908</v>
       </c>
       <c r="C126">
         <v>0</v>
@@ -3174,13 +3557,16 @@
       <c r="F126">
         <v>161996</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G126">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
         <v>5</v>
       </c>
-      <c r="B127">
-        <v>2012</v>
+      <c r="B127" s="2">
+        <v>41274</v>
       </c>
       <c r="C127">
         <v>2</v>
@@ -3194,13 +3580,16 @@
       <c r="F127">
         <v>212094</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G127">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
         <v>5</v>
       </c>
-      <c r="B128">
-        <v>2013</v>
+      <c r="B128" s="2">
+        <v>41639</v>
       </c>
       <c r="C128">
         <v>1</v>
@@ -3214,13 +3603,16 @@
       <c r="F128">
         <v>130219</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G128">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A129" t="s">
         <v>5</v>
       </c>
-      <c r="B129">
-        <v>2014</v>
+      <c r="B129" s="2">
+        <v>42004</v>
       </c>
       <c r="C129">
         <v>1</v>
@@ -3234,13 +3626,16 @@
       <c r="F129">
         <v>119867</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G129">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A130" t="s">
         <v>5</v>
       </c>
-      <c r="B130">
-        <v>2015</v>
+      <c r="B130" s="2">
+        <v>42369</v>
       </c>
       <c r="C130">
         <v>2</v>
@@ -3254,13 +3649,16 @@
       <c r="F130">
         <v>121386</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G130">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A131" t="s">
         <v>5</v>
       </c>
-      <c r="B131">
-        <v>2016</v>
+      <c r="B131" s="2">
+        <v>42735</v>
       </c>
       <c r="C131">
         <v>2</v>
@@ -3274,13 +3672,16 @@
       <c r="F131">
         <v>116135</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G131">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A132" t="s">
         <v>5</v>
       </c>
-      <c r="B132">
-        <v>2017</v>
+      <c r="B132" s="2">
+        <v>43100</v>
       </c>
       <c r="C132">
         <v>5</v>
@@ -3294,13 +3695,16 @@
       <c r="F132">
         <v>117824</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G132">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
         <v>5</v>
       </c>
-      <c r="B133">
-        <v>2018</v>
+      <c r="B133" s="2">
+        <v>43465</v>
       </c>
       <c r="C133">
         <v>3</v>
@@ -3314,13 +3718,16 @@
       <c r="F133">
         <v>118213</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G133">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A134" t="s">
         <v>5</v>
       </c>
-      <c r="B134">
-        <v>2019</v>
+      <c r="B134" s="2">
+        <v>43830</v>
       </c>
       <c r="C134">
         <v>7</v>
@@ -3334,13 +3741,16 @@
       <c r="F134">
         <v>104854</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G134">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A135" t="s">
         <v>5</v>
       </c>
-      <c r="B135">
-        <v>2020</v>
+      <c r="B135" s="2">
+        <v>44196</v>
       </c>
       <c r="C135">
         <v>2</v>
@@ -3354,13 +3764,16 @@
       <c r="F135">
         <v>105872</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G135">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A136" t="s">
         <v>5</v>
       </c>
-      <c r="B136">
-        <v>2021</v>
+      <c r="B136" s="2">
+        <v>44561</v>
       </c>
       <c r="C136">
         <v>4</v>
@@ -3374,13 +3787,16 @@
       <c r="F136">
         <v>120100</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G136">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A137" t="s">
         <v>5</v>
       </c>
-      <c r="B137">
-        <v>2022</v>
+      <c r="B137" s="2">
+        <v>44926</v>
       </c>
       <c r="C137">
         <v>3</v>
@@ -3394,13 +3810,16 @@
       <c r="F137">
         <v>101846</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G137">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A138" t="s">
         <v>14</v>
       </c>
-      <c r="B138">
-        <v>2006</v>
+      <c r="B138" s="2">
+        <v>39082</v>
       </c>
       <c r="C138">
         <v>4</v>
@@ -3414,13 +3833,16 @@
       <c r="F138">
         <v>32522</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G138">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A139" t="s">
         <v>14</v>
       </c>
-      <c r="B139">
-        <v>2007</v>
+      <c r="B139" s="2">
+        <v>39447</v>
       </c>
       <c r="C139">
         <v>2</v>
@@ -3434,13 +3856,16 @@
       <c r="F139">
         <v>81084</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G139">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A140" t="s">
         <v>14</v>
       </c>
-      <c r="B140">
-        <v>2008</v>
+      <c r="B140" s="2">
+        <v>39813</v>
       </c>
       <c r="C140">
         <v>3</v>
@@ -3454,13 +3879,16 @@
       <c r="F140">
         <v>94394</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G140">
+        <v>28.7</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A141" t="s">
         <v>14</v>
       </c>
-      <c r="B141">
-        <v>2009</v>
+      <c r="B141" s="2">
+        <v>40178</v>
       </c>
       <c r="C141">
         <v>4</v>
@@ -3474,13 +3902,16 @@
       <c r="F141">
         <v>104376</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G141">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A142" t="s">
         <v>14</v>
       </c>
-      <c r="B142">
-        <v>2010</v>
+      <c r="B142" s="2">
+        <v>40543</v>
       </c>
       <c r="C142">
         <v>1</v>
@@ -3494,13 +3925,16 @@
       <c r="F142">
         <v>130355</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G142">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A143" t="s">
         <v>14</v>
       </c>
-      <c r="B143">
-        <v>2011</v>
+      <c r="B143" s="2">
+        <v>40908</v>
       </c>
       <c r="C143">
         <v>3</v>
@@ -3514,13 +3948,16 @@
       <c r="F143">
         <v>168780</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G143">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A144" t="s">
         <v>14</v>
       </c>
-      <c r="B144">
-        <v>2012</v>
+      <c r="B144" s="2">
+        <v>41274</v>
       </c>
       <c r="C144">
         <v>0</v>
@@ -3534,13 +3971,16 @@
       <c r="F144">
         <v>211103</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G144">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A145" t="s">
         <v>14</v>
       </c>
-      <c r="B145">
-        <v>2013</v>
+      <c r="B145" s="2">
+        <v>41639</v>
       </c>
       <c r="C145">
         <v>1</v>
@@ -3554,13 +3994,16 @@
       <c r="F145">
         <v>154983</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G145">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A146" t="s">
         <v>14</v>
       </c>
-      <c r="B146">
-        <v>2014</v>
+      <c r="B146" s="2">
+        <v>42004</v>
       </c>
       <c r="C146">
         <v>4</v>
@@ -3574,13 +4017,16 @@
       <c r="F146">
         <v>104732</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G146">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A147" t="s">
         <v>14</v>
       </c>
-      <c r="B147">
-        <v>2015</v>
+      <c r="B147" s="2">
+        <v>42369</v>
       </c>
       <c r="C147">
         <v>4</v>
@@ -3594,13 +4040,16 @@
       <c r="F147">
         <v>79519</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G147">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A148" t="s">
         <v>14</v>
       </c>
-      <c r="B148">
-        <v>2016</v>
+      <c r="B148" s="2">
+        <v>42735</v>
       </c>
       <c r="C148">
         <v>2</v>
@@ -3614,13 +4063,16 @@
       <c r="F148">
         <v>70669</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G148">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A149" t="s">
         <v>14</v>
       </c>
-      <c r="B149">
-        <v>2017</v>
+      <c r="B149" s="2">
+        <v>43100</v>
       </c>
       <c r="C149">
         <v>5</v>
@@ -3634,13 +4086,16 @@
       <c r="F149">
         <v>78862</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G149">
+        <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A150" t="s">
         <v>14</v>
       </c>
-      <c r="B150">
-        <v>2018</v>
+      <c r="B150" s="2">
+        <v>43465</v>
       </c>
       <c r="C150">
         <v>5</v>
@@ -3654,13 +4109,16 @@
       <c r="F150">
         <v>91313</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G150">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A151" t="s">
         <v>14</v>
       </c>
-      <c r="B151">
-        <v>2019</v>
+      <c r="B151" s="2">
+        <v>43830</v>
       </c>
       <c r="C151">
         <v>6</v>
@@ -3674,13 +4132,16 @@
       <c r="F151">
         <v>91314</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G151">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A152" t="s">
         <v>14</v>
       </c>
-      <c r="B152">
-        <v>2020</v>
+      <c r="B152" s="2">
+        <v>44196</v>
       </c>
       <c r="C152">
         <v>9</v>
@@ -3694,13 +4155,16 @@
       <c r="F152">
         <v>101218</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G152">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A153" t="s">
         <v>14</v>
       </c>
-      <c r="B153">
-        <v>2021</v>
+      <c r="B153" s="2">
+        <v>44561</v>
       </c>
       <c r="C153">
         <v>13</v>
@@ -3714,13 +4178,16 @@
       <c r="F153">
         <v>126019</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G153">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A154" t="s">
         <v>14</v>
       </c>
-      <c r="B154">
-        <v>2022</v>
+      <c r="B154" s="2">
+        <v>44926</v>
       </c>
       <c r="C154">
         <v>5</v>
@@ -3734,13 +4201,16 @@
       <c r="F154">
         <v>118263</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G154">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A155" t="s">
         <v>15</v>
       </c>
-      <c r="B155">
-        <v>2006</v>
+      <c r="B155" s="2">
+        <v>39082</v>
       </c>
       <c r="C155">
         <v>7</v>
@@ -3754,13 +4224,16 @@
       <c r="F155">
         <v>76099</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G155">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A156" t="s">
         <v>15</v>
       </c>
-      <c r="B156">
-        <v>2007</v>
+      <c r="B156" s="2">
+        <v>39447</v>
       </c>
       <c r="C156">
         <v>7</v>
@@ -3774,13 +4247,16 @@
       <c r="F156">
         <v>87515</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G156">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A157" t="s">
         <v>15</v>
       </c>
-      <c r="B157">
-        <v>2008</v>
+      <c r="B157" s="2">
+        <v>39813</v>
       </c>
       <c r="C157">
         <v>15</v>
@@ -3794,13 +4270,16 @@
       <c r="F157">
         <v>172003</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G157">
+        <v>41.6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A158" t="s">
         <v>15</v>
       </c>
-      <c r="B158">
-        <v>2009</v>
+      <c r="B158" s="2">
+        <v>40178</v>
       </c>
       <c r="C158">
         <v>11</v>
@@ -3814,13 +4293,16 @@
       <c r="F158">
         <v>226563</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G158">
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A159" t="s">
         <v>15</v>
       </c>
-      <c r="B159">
-        <v>2010</v>
+      <c r="B159" s="2">
+        <v>40543</v>
       </c>
       <c r="C159">
         <v>7</v>
@@ -3834,13 +4316,16 @@
       <c r="F159">
         <v>257155</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G159">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A160" t="s">
         <v>15</v>
       </c>
-      <c r="B160">
-        <v>2011</v>
+      <c r="B160" s="2">
+        <v>40908</v>
       </c>
       <c r="C160">
         <v>8</v>
@@ -3854,13 +4339,16 @@
       <c r="F160">
         <v>210264</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G160">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A161" t="s">
         <v>15</v>
       </c>
-      <c r="B161">
-        <v>2012</v>
+      <c r="B161" s="2">
+        <v>41274</v>
       </c>
       <c r="C161">
         <v>16</v>
@@ -3874,13 +4362,16 @@
       <c r="F161">
         <v>213808</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G161">
+        <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A162" t="s">
         <v>15</v>
       </c>
-      <c r="B162">
-        <v>2013</v>
+      <c r="B162" s="2">
+        <v>41639</v>
       </c>
       <c r="C162">
         <v>11</v>
@@ -3894,13 +4385,16 @@
       <c r="F162">
         <v>195880</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G162">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A163" t="s">
         <v>15</v>
       </c>
-      <c r="B163">
-        <v>2014</v>
+      <c r="B163" s="2">
+        <v>42004</v>
       </c>
       <c r="C163">
         <v>13</v>
@@ -3914,13 +4408,16 @@
       <c r="F163">
         <v>138776</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G163">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A164" t="s">
         <v>15</v>
       </c>
-      <c r="B164">
-        <v>2015</v>
+      <c r="B164" s="2">
+        <v>42369</v>
       </c>
       <c r="C164">
         <v>9</v>
@@ -3934,13 +4431,16 @@
       <c r="F164">
         <v>84841</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G164">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A165" t="s">
         <v>15</v>
       </c>
-      <c r="B165">
-        <v>2016</v>
+      <c r="B165" s="2">
+        <v>42735</v>
       </c>
       <c r="C165">
         <v>15</v>
@@ -3954,13 +4454,16 @@
       <c r="F165">
         <v>120392</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G165">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A166" t="s">
         <v>15</v>
       </c>
-      <c r="B166">
-        <v>2017</v>
+      <c r="B166" s="2">
+        <v>43100</v>
       </c>
       <c r="C166">
         <v>24</v>
@@ -3974,13 +4477,16 @@
       <c r="F166">
         <v>120813</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G166">
+        <v>22.6</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A167" t="s">
         <v>15</v>
       </c>
-      <c r="B167">
-        <v>2018</v>
+      <c r="B167" s="2">
+        <v>43465</v>
       </c>
       <c r="C167">
         <v>30</v>
@@ -3994,13 +4500,16 @@
       <c r="F167">
         <v>122044</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G167">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A168" t="s">
         <v>15</v>
       </c>
-      <c r="B168">
-        <v>2019</v>
+      <c r="B168" s="2">
+        <v>43830</v>
       </c>
       <c r="C168">
         <v>15</v>
@@ -4014,13 +4523,16 @@
       <c r="F168">
         <v>138756</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G168">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A169" t="s">
         <v>15</v>
       </c>
-      <c r="B169">
-        <v>2020</v>
+      <c r="B169" s="2">
+        <v>44196</v>
       </c>
       <c r="C169">
         <v>22</v>
@@ -4034,13 +4546,16 @@
       <c r="F169">
         <v>147049</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G169">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A170" t="s">
         <v>15</v>
       </c>
-      <c r="B170">
-        <v>2021</v>
+      <c r="B170" s="2">
+        <v>44561</v>
       </c>
       <c r="C170">
         <v>27</v>
@@ -4054,13 +4569,16 @@
       <c r="F170">
         <v>173007</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G170">
+        <v>22.1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A171" t="s">
         <v>15</v>
       </c>
-      <c r="B171">
-        <v>2022</v>
+      <c r="B171" s="2">
+        <v>44926</v>
       </c>
       <c r="C171">
         <v>41</v>
@@ -4074,13 +4592,16 @@
       <c r="F171">
         <v>153457</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G171">
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A172" t="s">
         <v>16</v>
       </c>
-      <c r="B172">
-        <v>2006</v>
+      <c r="B172" s="2">
+        <v>39082</v>
       </c>
       <c r="C172">
         <v>7</v>
@@ -4094,13 +4615,16 @@
       <c r="F172">
         <v>73044</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G172">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A173" t="s">
         <v>16</v>
       </c>
-      <c r="B173">
-        <v>2007</v>
+      <c r="B173" s="2">
+        <v>39447</v>
       </c>
       <c r="C173">
         <v>7</v>
@@ -4114,13 +4638,16 @@
       <c r="F173">
         <v>106354</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G173">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A174" t="s">
         <v>16</v>
       </c>
-      <c r="B174">
-        <v>2008</v>
+      <c r="B174" s="2">
+        <v>39813</v>
       </c>
       <c r="C174">
         <v>27</v>
@@ -4134,13 +4661,16 @@
       <c r="F174">
         <v>120175</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G174">
+        <v>41.6</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A175" t="s">
         <v>16</v>
       </c>
-      <c r="B175">
-        <v>2009</v>
+      <c r="B175" s="2">
+        <v>40178</v>
       </c>
       <c r="C175">
         <v>24</v>
@@ -4154,13 +4684,16 @@
       <c r="F175">
         <v>144081</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G175">
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A176" t="s">
         <v>16</v>
       </c>
-      <c r="B176">
-        <v>2010</v>
+      <c r="B176" s="2">
+        <v>40543</v>
       </c>
       <c r="C176">
         <v>8</v>
@@ -4174,13 +4707,16 @@
       <c r="F176">
         <v>161462</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G176">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A177" t="s">
         <v>16</v>
       </c>
-      <c r="B177">
-        <v>2011</v>
+      <c r="B177" s="2">
+        <v>40908</v>
       </c>
       <c r="C177">
         <v>11</v>
@@ -4194,13 +4730,16 @@
       <c r="F177">
         <v>180756</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G177">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A178" t="s">
         <v>16</v>
       </c>
-      <c r="B178">
-        <v>2012</v>
+      <c r="B178" s="2">
+        <v>41274</v>
       </c>
       <c r="C178">
         <v>8</v>
@@ -4214,13 +4753,16 @@
       <c r="F178">
         <v>221410</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G178">
+        <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A179" t="s">
         <v>16</v>
       </c>
-      <c r="B179">
-        <v>2013</v>
+      <c r="B179" s="2">
+        <v>41639</v>
       </c>
       <c r="C179">
         <v>5</v>
@@ -4234,13 +4776,16 @@
       <c r="F179">
         <v>309678</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G179">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A180" t="s">
         <v>16</v>
       </c>
-      <c r="B180">
-        <v>2014</v>
+      <c r="B180" s="2">
+        <v>42004</v>
       </c>
       <c r="C180">
         <v>2</v>
@@ -4254,13 +4799,16 @@
       <c r="F180">
         <v>129508</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G180">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A181" t="s">
         <v>16</v>
       </c>
-      <c r="B181">
-        <v>2015</v>
+      <c r="B181" s="2">
+        <v>42369</v>
       </c>
       <c r="C181">
         <v>8</v>
@@ -4274,13 +4822,16 @@
       <c r="F181">
         <v>130516</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G181">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A182" t="s">
         <v>16</v>
       </c>
-      <c r="B182">
-        <v>2016</v>
+      <c r="B182" s="2">
+        <v>42735</v>
       </c>
       <c r="C182">
         <v>5</v>
@@ -4294,13 +4845,16 @@
       <c r="F182">
         <v>135068</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G182">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A183" t="s">
         <v>16</v>
       </c>
-      <c r="B183">
-        <v>2017</v>
+      <c r="B183" s="2">
+        <v>43100</v>
       </c>
       <c r="C183">
         <v>17</v>
@@ -4314,13 +4868,16 @@
       <c r="F183">
         <v>135267</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G183">
+        <v>22.6</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A184" t="s">
         <v>16</v>
       </c>
-      <c r="B184">
-        <v>2018</v>
+      <c r="B184" s="2">
+        <v>43465</v>
       </c>
       <c r="C184">
         <v>10</v>
@@ -4334,13 +4891,16 @@
       <c r="F184">
         <v>86774</v>
       </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G184">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A185" t="s">
         <v>16</v>
       </c>
-      <c r="B185">
-        <v>2019</v>
+      <c r="B185" s="2">
+        <v>43830</v>
       </c>
       <c r="C185">
         <v>10</v>
@@ -4354,13 +4914,16 @@
       <c r="F185">
         <v>65957</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G185">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A186" t="s">
         <v>16</v>
       </c>
-      <c r="B186">
-        <v>2020</v>
+      <c r="B186" s="2">
+        <v>44196</v>
       </c>
       <c r="C186">
         <v>4</v>
@@ -4374,13 +4937,16 @@
       <c r="F186">
         <v>78764</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G186">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A187" t="s">
         <v>16</v>
       </c>
-      <c r="B187">
-        <v>2021</v>
+      <c r="B187" s="2">
+        <v>44561</v>
       </c>
       <c r="C187">
         <v>17</v>
@@ -4394,13 +4960,16 @@
       <c r="F187">
         <v>80948</v>
       </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G187">
+        <v>22.1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A188" t="s">
         <v>16</v>
       </c>
-      <c r="B188">
-        <v>2022</v>
+      <c r="B188" s="2">
+        <v>44926</v>
       </c>
       <c r="C188">
         <v>11</v>
@@ -4414,13 +4983,16 @@
       <c r="F188">
         <v>56752</v>
       </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G188">
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A189" t="s">
         <v>11</v>
       </c>
-      <c r="B189">
-        <v>2006</v>
+      <c r="B189" s="2">
+        <v>39082</v>
       </c>
       <c r="C189">
         <v>2</v>
@@ -4434,13 +5006,16 @@
       <c r="F189">
         <v>65815</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G189">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A190" t="s">
         <v>11</v>
       </c>
-      <c r="B190">
-        <v>2007</v>
+      <c r="B190" s="2">
+        <v>39447</v>
       </c>
       <c r="C190">
         <v>1</v>
@@ -4454,13 +5029,16 @@
       <c r="F190">
         <v>75078</v>
       </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G190">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A191" t="s">
         <v>11</v>
       </c>
-      <c r="B191">
-        <v>2008</v>
+      <c r="B191" s="2">
+        <v>39813</v>
       </c>
       <c r="C191">
         <v>3</v>
@@ -4474,13 +5052,16 @@
       <c r="F191">
         <v>104988</v>
       </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G191">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A192" t="s">
         <v>11</v>
       </c>
-      <c r="B192">
-        <v>2009</v>
+      <c r="B192" s="2">
+        <v>40178</v>
       </c>
       <c r="C192">
         <v>5</v>
@@ -4494,13 +5075,16 @@
       <c r="F192">
         <v>105626</v>
       </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G192">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A193" t="s">
         <v>11</v>
       </c>
-      <c r="B193">
-        <v>2010</v>
+      <c r="B193" s="2">
+        <v>40543</v>
       </c>
       <c r="C193">
         <v>1</v>
@@ -4514,13 +5098,16 @@
       <c r="F193">
         <v>136254</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G193">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A194" t="s">
         <v>11</v>
       </c>
-      <c r="B194">
-        <v>2011</v>
+      <c r="B194" s="2">
+        <v>40908</v>
       </c>
       <c r="C194">
         <v>1</v>
@@ -4534,13 +5121,16 @@
       <c r="F194">
         <v>141726</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G194">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A195" t="s">
         <v>11</v>
       </c>
-      <c r="B195">
-        <v>2012</v>
+      <c r="B195" s="2">
+        <v>41274</v>
       </c>
       <c r="C195">
         <v>0</v>
@@ -4554,13 +5144,16 @@
       <c r="F195">
         <v>145018</v>
       </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G195">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A196" t="s">
         <v>11</v>
       </c>
-      <c r="B196">
-        <v>2013</v>
+      <c r="B196" s="2">
+        <v>41639</v>
       </c>
       <c r="C196">
         <v>9</v>
@@ -4574,13 +5167,16 @@
       <c r="F196">
         <v>132259</v>
       </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G196">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A197" t="s">
         <v>11</v>
       </c>
-      <c r="B197">
-        <v>2014</v>
+      <c r="B197" s="2">
+        <v>42004</v>
       </c>
       <c r="C197">
         <v>6</v>
@@ -4594,13 +5190,16 @@
       <c r="F197">
         <v>93945</v>
       </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G197">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A198" t="s">
         <v>11</v>
       </c>
-      <c r="B198">
-        <v>2015</v>
+      <c r="B198" s="2">
+        <v>42369</v>
       </c>
       <c r="C198">
         <v>8</v>
@@ -4614,13 +5213,16 @@
       <c r="F198">
         <v>106550</v>
       </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G198">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A199" t="s">
         <v>11</v>
       </c>
-      <c r="B199">
-        <v>2016</v>
+      <c r="B199" s="2">
+        <v>42735</v>
       </c>
       <c r="C199">
         <v>5</v>
@@ -4634,13 +5236,16 @@
       <c r="F199">
         <v>134448</v>
       </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G199">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A200" t="s">
         <v>11</v>
       </c>
-      <c r="B200">
-        <v>2017</v>
+      <c r="B200" s="2">
+        <v>43100</v>
       </c>
       <c r="C200">
         <v>5</v>
@@ -4654,13 +5259,16 @@
       <c r="F200">
         <v>170242</v>
       </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G200">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A201" t="s">
         <v>11</v>
       </c>
-      <c r="B201">
-        <v>2018</v>
+      <c r="B201" s="2">
+        <v>43465</v>
       </c>
       <c r="C201">
         <v>12</v>
@@ -4674,13 +5282,16 @@
       <c r="F201">
         <v>150731</v>
       </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G201">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A202" t="s">
         <v>11</v>
       </c>
-      <c r="B202">
-        <v>2019</v>
+      <c r="B202" s="2">
+        <v>43830</v>
       </c>
       <c r="C202">
         <v>6</v>
@@ -4694,13 +5305,16 @@
       <c r="F202">
         <v>146864</v>
       </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G202">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A203" t="s">
         <v>11</v>
       </c>
-      <c r="B203">
-        <v>2020</v>
+      <c r="B203" s="2">
+        <v>44196</v>
       </c>
       <c r="C203">
         <v>13</v>
@@ -4714,13 +5328,16 @@
       <c r="F203">
         <v>149449</v>
       </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G203">
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A204" t="s">
         <v>11</v>
       </c>
-      <c r="B204">
-        <v>2021</v>
+      <c r="B204" s="2">
+        <v>44561</v>
       </c>
       <c r="C204">
         <v>28</v>
@@ -4734,13 +5351,16 @@
       <c r="F204">
         <v>182753</v>
       </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G204">
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A205" t="s">
         <v>11</v>
       </c>
-      <c r="B205">
-        <v>2022</v>
+      <c r="B205" s="2">
+        <v>44926</v>
       </c>
       <c r="C205">
         <v>31</v>
@@ -4754,13 +5374,16 @@
       <c r="F205">
         <v>113889</v>
       </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G205">
+        <v>19.7</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A206" t="s">
         <v>10</v>
       </c>
-      <c r="B206">
-        <v>2006</v>
+      <c r="B206" s="2">
+        <v>39082</v>
       </c>
       <c r="C206">
         <v>0</v>
@@ -4774,13 +5397,16 @@
       <c r="F206">
         <v>4858</v>
       </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G206">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A207" t="s">
         <v>10</v>
       </c>
-      <c r="B207">
-        <v>2007</v>
+      <c r="B207" s="2">
+        <v>39447</v>
       </c>
       <c r="C207">
         <v>0</v>
@@ -4794,13 +5420,16 @@
       <c r="F207">
         <v>7334</v>
       </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G207">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A208" t="s">
         <v>10</v>
       </c>
-      <c r="B208">
-        <v>2008</v>
+      <c r="B208" s="2">
+        <v>39813</v>
       </c>
       <c r="C208">
         <v>0</v>
@@ -4814,13 +5443,16 @@
       <c r="F208">
         <v>9458</v>
       </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G208">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A209" t="s">
         <v>10</v>
       </c>
-      <c r="B209">
-        <v>2009</v>
+      <c r="B209" s="2">
+        <v>40178</v>
       </c>
       <c r="C209">
         <v>1</v>
@@ -4834,13 +5466,16 @@
       <c r="F209">
         <v>11163</v>
       </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G209">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A210" t="s">
         <v>10</v>
       </c>
-      <c r="B210">
-        <v>2010</v>
+      <c r="B210" s="2">
+        <v>40543</v>
       </c>
       <c r="C210">
         <v>0</v>
@@ -4854,13 +5489,16 @@
       <c r="F210">
         <v>18071</v>
       </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G210">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A211" t="s">
         <v>10</v>
       </c>
-      <c r="B211">
-        <v>2011</v>
+      <c r="B211" s="2">
+        <v>40908</v>
       </c>
       <c r="C211">
         <v>0</v>
@@ -4874,13 +5512,16 @@
       <c r="F211">
         <v>18971</v>
       </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G211">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A212" t="s">
         <v>10</v>
       </c>
-      <c r="B212">
-        <v>2012</v>
+      <c r="B212" s="2">
+        <v>41274</v>
       </c>
       <c r="C212">
         <v>0</v>
@@ -4894,13 +5535,16 @@
       <c r="F212">
         <v>45194</v>
       </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A213" t="s">
         <v>10</v>
       </c>
-      <c r="B213">
-        <v>2013</v>
+      <c r="B213" s="2">
+        <v>41639</v>
       </c>
       <c r="C213">
         <v>2</v>
@@ -4914,13 +5558,16 @@
       <c r="F213">
         <v>50895</v>
       </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G213">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A214" t="s">
         <v>10</v>
       </c>
-      <c r="B214">
-        <v>2014</v>
+      <c r="B214" s="2">
+        <v>42004</v>
       </c>
       <c r="C214">
         <v>0</v>
@@ -4934,13 +5581,16 @@
       <c r="F214">
         <v>66480</v>
       </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A215" t="s">
         <v>10</v>
       </c>
-      <c r="B215">
-        <v>2015</v>
+      <c r="B215" s="2">
+        <v>42369</v>
       </c>
       <c r="C215">
         <v>1</v>
@@ -4954,13 +5604,16 @@
       <c r="F215">
         <v>29839</v>
       </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A216" t="s">
         <v>10</v>
       </c>
-      <c r="B216">
-        <v>2016</v>
+      <c r="B216" s="2">
+        <v>42735</v>
       </c>
       <c r="C216">
         <v>1</v>
@@ -4974,13 +5627,16 @@
       <c r="F216">
         <v>44988</v>
       </c>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G216">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A217" t="s">
         <v>10</v>
       </c>
-      <c r="B217">
-        <v>2017</v>
+      <c r="B217" s="2">
+        <v>43100</v>
       </c>
       <c r="C217">
         <v>2</v>
@@ -4994,13 +5650,16 @@
       <c r="F217">
         <v>36354</v>
       </c>
-    </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G217">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A218" t="s">
         <v>10</v>
       </c>
-      <c r="B218">
-        <v>2018</v>
+      <c r="B218" s="2">
+        <v>43465</v>
       </c>
       <c r="C218">
         <v>2</v>
@@ -5014,13 +5673,16 @@
       <c r="F218">
         <v>37684</v>
       </c>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G218">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A219" t="s">
         <v>10</v>
       </c>
-      <c r="B219">
-        <v>2019</v>
+      <c r="B219" s="2">
+        <v>43830</v>
       </c>
       <c r="C219">
         <v>0</v>
@@ -5034,13 +5696,16 @@
       <c r="F219">
         <v>44556</v>
       </c>
-    </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G219">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A220" t="s">
         <v>10</v>
       </c>
-      <c r="B220">
-        <v>2020</v>
+      <c r="B220" s="2">
+        <v>44196</v>
       </c>
       <c r="C220">
         <v>2</v>
@@ -5054,13 +5719,16 @@
       <c r="F220">
         <v>55578</v>
       </c>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A221" t="s">
         <v>10</v>
       </c>
-      <c r="B221">
-        <v>2021</v>
+      <c r="B221" s="2">
+        <v>44561</v>
       </c>
       <c r="C221">
         <v>3</v>
@@ -5074,13 +5742,16 @@
       <c r="F221">
         <v>85231</v>
       </c>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G221">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A222" t="s">
         <v>10</v>
       </c>
-      <c r="B222">
-        <v>2022</v>
+      <c r="B222" s="2">
+        <v>44926</v>
       </c>
       <c r="C222">
         <v>0</v>
@@ -5093,6 +5764,9 @@
       </c>
       <c r="F222">
         <v>117602</v>
+      </c>
+      <c r="G222">
+        <v>3.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>